<commit_message>
changes - boq list added to spreadsheet
</commit_message>
<xml_diff>
--- a/testproject.xlsx
+++ b/testproject.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamp\Desktop\codeworkspace\github\greensheet_interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA34F708-F9B0-4A06-87C4-D9862D2A423A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EA4D0E-8335-4179-A23E-B96CB8BB52B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Greensheet" sheetId="1" r:id="rId1"/>
     <sheet name="Project Budget (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Greensheet!$A$1:$AE$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Greensheet!$A$1:$AE$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Project Budget (2)'!$A$1:$S$32</definedName>
-    <definedName name="VAR__1_1_1_1" localSheetId="0">Greensheet!$C$4:$C$4,Greensheet!#REF!</definedName>
+    <definedName name="VAR__1_1_1_1" localSheetId="0">Greensheet!$C$5:$C$5,Greensheet!#REF!</definedName>
     <definedName name="VAR__1_1_1_1" localSheetId="1">'Project Budget (2)'!$C$4:$C$4,'Project Budget (2)'!#REF!</definedName>
-    <definedName name="VAR__1_1_1_2" localSheetId="0">Greensheet!$D$4:$D$4,Greensheet!#REF!</definedName>
+    <definedName name="VAR__1_1_1_2" localSheetId="0">Greensheet!$D$5:$D$5,Greensheet!#REF!</definedName>
     <definedName name="VAR__1_1_1_2" localSheetId="1">'Project Budget (2)'!$D$4:$D$4,'Project Budget (2)'!#REF!</definedName>
-    <definedName name="VAR__1_1_1_3" localSheetId="0">Greensheet!$E$4:$E$4,Greensheet!#REF!</definedName>
+    <definedName name="VAR__1_1_1_3" localSheetId="0">Greensheet!$E$5:$E$5,Greensheet!#REF!</definedName>
     <definedName name="VAR__1_1_1_3" localSheetId="1">'Project Budget (2)'!$E$4:$E$4,'Project Budget (2)'!#REF!</definedName>
-    <definedName name="VAR__1_1_1_4" localSheetId="0">Greensheet!$F$4:$F$4,Greensheet!#REF!</definedName>
+    <definedName name="VAR__1_1_1_4" localSheetId="0">Greensheet!$F$5:$F$5,Greensheet!#REF!</definedName>
     <definedName name="VAR__1_1_1_4" localSheetId="1">'Project Budget (2)'!$F$4:$F$4,'Project Budget (2)'!#REF!</definedName>
     <definedName name="VAR__1_1_1_5" localSheetId="0">Greensheet!#REF!,Greensheet!#REF!</definedName>
     <definedName name="VAR__1_1_1_5" localSheetId="1">'Project Budget (2)'!#REF!,'Project Budget (2)'!#REF!</definedName>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
   <si>
     <t>21.19L - Rock Mountain TARG CWB</t>
   </si>
@@ -250,10 +250,16 @@
     <t>LF</t>
   </si>
   <si>
-    <t>&lt;-- Job Number</t>
+    <t>J420</t>
   </si>
   <si>
-    <t>J420</t>
+    <t>&lt;-- Job Number (Income)</t>
+  </si>
+  <si>
+    <t>&lt;-- Job Number (Costs)</t>
+  </si>
+  <si>
+    <t>J374</t>
   </si>
 </sst>
 </file>
@@ -871,7 +877,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="81">
+  <borders count="85">
     <border>
       <left/>
       <right/>
@@ -1715,60 +1721,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1903,6 +1855,98 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -2292,7 +2336,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2892,23 +2936,17 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="53" fillId="8" borderId="66" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="53" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="34" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="53" fillId="34" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="35" borderId="72" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="35" borderId="68" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="53" fillId="7" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2932,77 +2970,105 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="34" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="53" fillId="34" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="53" fillId="34" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="53" fillId="7" borderId="74" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="53" fillId="7" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="53" fillId="7" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="53" fillId="7" borderId="75" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="9" borderId="72" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="53" fillId="7" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="9" borderId="68" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="29" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="34" borderId="77" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="34" borderId="73" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="34" borderId="78" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="34" borderId="77" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="1" fillId="34" borderId="74" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="34" borderId="73" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="34" borderId="77" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="34" borderId="79" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="34" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="1" fillId="34" borderId="73" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="34" borderId="75" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="34" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="53" fillId="34" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="53" fillId="34" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="1" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="35" borderId="66" xfId="12" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="35" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="53" fillId="35" borderId="70" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="35" borderId="66" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="35" borderId="58" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="35" borderId="79" xfId="12" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="35" borderId="80" xfId="12" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="35" borderId="81" xfId="12" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="35" borderId="21" xfId="12" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="35" borderId="77" xfId="12" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="35" borderId="58" xfId="12" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="53" fillId="8" borderId="82" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="53" fillId="8" borderId="83" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="7" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="7" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="6" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3015,9 +3081,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="35" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3575,11 +3638,11 @@
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AG30"/>
+  <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" customHeight="1"/>
@@ -3596,797 +3659,740 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="21" customHeight="1">
-      <c r="A1" s="225" t="s">
+      <c r="A1" s="209" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="208" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="210" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="211" t="s">
+      <c r="C1" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="212"/>
-      <c r="E1" s="212"/>
-      <c r="F1" s="213"/>
-      <c r="G1" s="181">
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
+      <c r="F1" s="216"/>
+      <c r="G1" s="220">
         <v>43556</v>
       </c>
-      <c r="H1" s="181">
+      <c r="H1" s="220">
         <v>43586</v>
       </c>
-      <c r="I1" s="181">
+      <c r="I1" s="220">
         <v>43617</v>
       </c>
-      <c r="J1" s="181">
+      <c r="J1" s="220">
         <v>43647</v>
       </c>
-      <c r="K1" s="181">
+      <c r="K1" s="220">
         <v>43678</v>
       </c>
-      <c r="L1" s="181">
+      <c r="L1" s="220">
         <v>43709</v>
       </c>
-      <c r="M1" s="181">
+      <c r="M1" s="220">
         <v>43739</v>
       </c>
-      <c r="N1" s="181">
+      <c r="N1" s="220">
         <v>43770</v>
       </c>
-      <c r="O1" s="181">
+      <c r="O1" s="220">
         <v>43800</v>
       </c>
-      <c r="P1" s="181">
+      <c r="P1" s="220">
         <v>43831</v>
       </c>
-      <c r="Q1" s="181">
+      <c r="Q1" s="220">
         <v>43862</v>
       </c>
-      <c r="R1" s="181">
+      <c r="R1" s="220">
         <v>43891</v>
       </c>
-      <c r="S1" s="181">
+      <c r="S1" s="220">
         <v>43922</v>
       </c>
-      <c r="T1" s="181">
+      <c r="T1" s="220">
         <v>43952</v>
       </c>
-      <c r="U1" s="181">
+      <c r="U1" s="220">
         <v>43983</v>
       </c>
-      <c r="V1" s="181">
+      <c r="V1" s="220">
         <v>44013</v>
       </c>
-      <c r="W1" s="181">
+      <c r="W1" s="220">
         <v>44044</v>
       </c>
-      <c r="X1" s="181">
+      <c r="X1" s="220">
         <v>44075</v>
       </c>
-      <c r="Y1" s="181">
+      <c r="Y1" s="220">
         <v>44105</v>
       </c>
-      <c r="Z1" s="181">
+      <c r="Z1" s="220">
         <v>44136</v>
       </c>
-      <c r="AA1" s="181">
+      <c r="AA1" s="220">
         <v>44166</v>
       </c>
-      <c r="AB1" s="181">
+      <c r="AB1" s="220">
         <v>44197</v>
       </c>
-      <c r="AC1" s="181">
+      <c r="AC1" s="220">
         <v>44228</v>
       </c>
-      <c r="AD1" s="181">
+      <c r="AD1" s="220">
         <v>44256</v>
       </c>
-      <c r="AE1" s="182" t="s">
+      <c r="AE1" s="222" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="A2" s="216" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="217"/>
-      <c r="C2" s="72" t="s">
+    <row r="2" spans="1:33" ht="21" customHeight="1">
+      <c r="A2" s="209" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="208" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="217"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="218"/>
+      <c r="F2" s="219"/>
+      <c r="G2" s="221"/>
+      <c r="H2" s="221"/>
+      <c r="I2" s="221"/>
+      <c r="J2" s="221"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
+      <c r="M2" s="221"/>
+      <c r="N2" s="221"/>
+      <c r="O2" s="221"/>
+      <c r="P2" s="221"/>
+      <c r="Q2" s="221"/>
+      <c r="R2" s="221"/>
+      <c r="S2" s="221"/>
+      <c r="T2" s="221"/>
+      <c r="U2" s="221"/>
+      <c r="V2" s="221"/>
+      <c r="W2" s="221"/>
+      <c r="X2" s="221"/>
+      <c r="Y2" s="221"/>
+      <c r="Z2" s="221"/>
+      <c r="AA2" s="221"/>
+      <c r="AB2" s="221"/>
+      <c r="AC2" s="221"/>
+      <c r="AD2" s="221"/>
+      <c r="AE2" s="223"/>
+    </row>
+    <row r="3" spans="1:33" s="3" customFormat="1" ht="21" customHeight="1">
+      <c r="A3" s="212" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="213"/>
+      <c r="C3" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="72" t="s">
+      <c r="D3" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="72" t="s">
+      <c r="E3" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="73" t="s">
+      <c r="F3" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="74" t="s">
+      <c r="G3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="74" t="s">
+      <c r="I3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="74" t="s">
+      <c r="J3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="74" t="s">
+      <c r="K3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="74" t="s">
+      <c r="L3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="74" t="s">
+      <c r="M3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="74" t="s">
+      <c r="N3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="74" t="s">
+      <c r="O3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="74" t="s">
+      <c r="P3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="74" t="s">
+      <c r="Q3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="74" t="s">
+      <c r="R3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="74" t="s">
+      <c r="S3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="74" t="s">
+      <c r="T3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="74" t="s">
+      <c r="U3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="74" t="s">
+      <c r="V3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="74" t="s">
+      <c r="W3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="X2" s="74" t="s">
+      <c r="X3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="Y2" s="74" t="s">
+      <c r="Y3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="Z2" s="74" t="s">
+      <c r="Z3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="74" t="s">
+      <c r="AA3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="74" t="s">
+      <c r="AB3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="AC2" s="74" t="s">
+      <c r="AC3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="AD2" s="74" t="s">
+      <c r="AD3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="AE2" s="183" t="s">
+      <c r="AE3" s="181" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" ht="21" customHeight="1">
-      <c r="A3" s="184"/>
-      <c r="B3" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="214"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="75"/>
-      <c r="R3" s="75"/>
-      <c r="S3" s="75"/>
-      <c r="T3" s="75"/>
-      <c r="U3" s="75"/>
-      <c r="V3" s="75"/>
-      <c r="W3" s="75"/>
-      <c r="X3" s="75"/>
-      <c r="Y3" s="75"/>
-      <c r="Z3" s="75"/>
-      <c r="AA3" s="75"/>
-      <c r="AB3" s="75"/>
-      <c r="AC3" s="75"/>
-      <c r="AD3" s="75"/>
-      <c r="AE3" s="185"/>
     </row>
     <row r="4" spans="1:33" ht="21" customHeight="1">
-      <c r="A4" s="186"/>
-      <c r="B4" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="76">
-        <v>0</v>
-      </c>
-      <c r="D4" s="77">
-        <v>0</v>
-      </c>
-      <c r="E4" s="78">
-        <f>SUM(C4:D4)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="79">
-        <f>SUMIFS($G4:$R4,$G$2:$R$2,"Actuals")</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="80">
-        <v>0</v>
-      </c>
-      <c r="H4" s="81">
-        <v>0</v>
-      </c>
-      <c r="I4" s="81">
-        <v>0</v>
-      </c>
-      <c r="J4" s="81">
-        <v>0</v>
-      </c>
-      <c r="K4" s="81">
-        <v>0</v>
-      </c>
-      <c r="L4" s="81">
-        <v>0</v>
-      </c>
-      <c r="M4" s="81">
-        <v>0</v>
-      </c>
-      <c r="N4" s="81">
-        <v>0</v>
-      </c>
-      <c r="O4" s="81">
-        <v>0</v>
-      </c>
-      <c r="P4" s="81">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="81">
-        <v>0</v>
-      </c>
-      <c r="R4" s="81">
-        <v>0</v>
-      </c>
-      <c r="S4" s="81">
-        <v>0</v>
-      </c>
-      <c r="T4" s="81">
-        <v>0</v>
-      </c>
-      <c r="U4" s="81">
-        <v>0</v>
-      </c>
-      <c r="V4" s="81">
-        <v>0</v>
-      </c>
-      <c r="W4" s="81">
-        <v>0</v>
-      </c>
-      <c r="X4" s="81">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="81">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="81">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="81">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="81">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="81">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="81">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="187">
-        <f>SUM(G4:R4)</f>
-        <v>0</v>
-      </c>
-      <c r="AF4" s="82"/>
+      <c r="A4" s="182"/>
+      <c r="B4" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="210"/>
+      <c r="D4" s="211"/>
+      <c r="E4" s="211"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="75"/>
+      <c r="P4" s="75"/>
+      <c r="Q4" s="75"/>
+      <c r="R4" s="75"/>
+      <c r="S4" s="75"/>
+      <c r="T4" s="75"/>
+      <c r="U4" s="75"/>
+      <c r="V4" s="75"/>
+      <c r="W4" s="75"/>
+      <c r="X4" s="75"/>
+      <c r="Y4" s="75"/>
+      <c r="Z4" s="75"/>
+      <c r="AA4" s="75"/>
+      <c r="AB4" s="75"/>
+      <c r="AC4" s="75"/>
+      <c r="AD4" s="75"/>
+      <c r="AE4" s="183"/>
     </row>
     <row r="5" spans="1:33" ht="21" customHeight="1">
-      <c r="A5" s="186"/>
-      <c r="B5" s="67"/>
+      <c r="A5" s="184"/>
+      <c r="B5" s="68" t="s">
+        <v>10</v>
+      </c>
       <c r="C5" s="76">
         <v>0</v>
       </c>
-      <c r="D5" s="83">
-        <v>0</v>
-      </c>
-      <c r="E5" s="76">
+      <c r="D5" s="77">
+        <v>0</v>
+      </c>
+      <c r="E5" s="78">
         <f>SUM(C5:D5)</f>
         <v>0</v>
       </c>
       <c r="F5" s="79">
-        <f>SUMIFS($G5:$R5,$G$2:$R$2,"Actuals")</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="84">
-        <v>0</v>
-      </c>
-      <c r="H5" s="85">
-        <v>0</v>
-      </c>
-      <c r="I5" s="85">
-        <v>0</v>
-      </c>
-      <c r="J5" s="85">
-        <v>0</v>
-      </c>
-      <c r="K5" s="85">
-        <v>0</v>
-      </c>
-      <c r="L5" s="85">
-        <v>0</v>
-      </c>
-      <c r="M5" s="85">
-        <v>0</v>
-      </c>
-      <c r="N5" s="85">
-        <v>0</v>
-      </c>
-      <c r="O5" s="85">
-        <v>0</v>
-      </c>
-      <c r="P5" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="85">
-        <v>0</v>
-      </c>
-      <c r="R5" s="85">
-        <v>0</v>
-      </c>
-      <c r="S5" s="85">
-        <v>0</v>
-      </c>
-      <c r="T5" s="85">
-        <v>0</v>
-      </c>
-      <c r="U5" s="85">
-        <v>0</v>
-      </c>
-      <c r="V5" s="85">
-        <v>0</v>
-      </c>
-      <c r="W5" s="85">
-        <v>0</v>
-      </c>
-      <c r="X5" s="85">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="85">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="85">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="85">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="85">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="85">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="85">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="187">
+        <f>SUMIFS($G5:$R5,$G$3:$R$3,"Actuals")</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="80">
+        <v>0</v>
+      </c>
+      <c r="H5" s="81">
+        <v>0</v>
+      </c>
+      <c r="I5" s="81">
+        <v>0</v>
+      </c>
+      <c r="J5" s="81">
+        <v>0</v>
+      </c>
+      <c r="K5" s="81">
+        <v>0</v>
+      </c>
+      <c r="L5" s="81">
+        <v>0</v>
+      </c>
+      <c r="M5" s="81">
+        <v>0</v>
+      </c>
+      <c r="N5" s="81">
+        <v>0</v>
+      </c>
+      <c r="O5" s="81">
+        <v>0</v>
+      </c>
+      <c r="P5" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="81">
+        <v>0</v>
+      </c>
+      <c r="R5" s="81">
+        <v>0</v>
+      </c>
+      <c r="S5" s="81">
+        <v>0</v>
+      </c>
+      <c r="T5" s="81">
+        <v>0</v>
+      </c>
+      <c r="U5" s="81">
+        <v>0</v>
+      </c>
+      <c r="V5" s="81">
+        <v>0</v>
+      </c>
+      <c r="W5" s="81">
+        <v>0</v>
+      </c>
+      <c r="X5" s="81">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="81">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="81">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="81">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="81">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="81">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="81">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="185">
         <f>SUM(G5:R5)</f>
         <v>0</v>
       </c>
       <c r="AF5" s="82"/>
     </row>
     <row r="6" spans="1:33" ht="21" customHeight="1">
-      <c r="A6" s="186"/>
-      <c r="B6" s="68"/>
+      <c r="A6" s="184"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="76">
         <v>0</v>
       </c>
-      <c r="D6" s="86">
-        <v>0</v>
-      </c>
-      <c r="E6" s="87">
+      <c r="D6" s="83">
+        <v>0</v>
+      </c>
+      <c r="E6" s="76">
         <f>SUM(C6:D6)</f>
         <v>0</v>
       </c>
       <c r="F6" s="79">
-        <f>SUMIFS($G6:$R6,$G$2:$R$2,"Actuals")</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="88">
-        <v>0</v>
-      </c>
-      <c r="H6" s="89">
-        <v>0</v>
-      </c>
-      <c r="I6" s="89">
-        <v>0</v>
-      </c>
-      <c r="J6" s="89">
-        <v>0</v>
-      </c>
-      <c r="K6" s="89">
-        <v>0</v>
-      </c>
-      <c r="L6" s="89">
-        <v>0</v>
-      </c>
-      <c r="M6" s="89">
-        <v>0</v>
-      </c>
-      <c r="N6" s="89">
-        <v>0</v>
-      </c>
-      <c r="O6" s="89">
-        <v>0</v>
-      </c>
-      <c r="P6" s="89">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="89">
-        <v>0</v>
-      </c>
-      <c r="R6" s="89">
-        <v>0</v>
-      </c>
-      <c r="S6" s="89">
-        <v>0</v>
-      </c>
-      <c r="T6" s="89">
-        <v>0</v>
-      </c>
-      <c r="U6" s="89">
-        <v>0</v>
-      </c>
-      <c r="V6" s="89">
-        <v>0</v>
-      </c>
-      <c r="W6" s="89">
-        <v>0</v>
-      </c>
-      <c r="X6" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="89">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="89">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="89">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="89">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="89">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="89">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="187">
+        <f>SUMIFS($G6:$R6,$G$3:$R$3,"Actuals")</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="84">
+        <v>0</v>
+      </c>
+      <c r="H6" s="85">
+        <v>0</v>
+      </c>
+      <c r="I6" s="85">
+        <v>0</v>
+      </c>
+      <c r="J6" s="85">
+        <v>0</v>
+      </c>
+      <c r="K6" s="85">
+        <v>0</v>
+      </c>
+      <c r="L6" s="85">
+        <v>0</v>
+      </c>
+      <c r="M6" s="85">
+        <v>0</v>
+      </c>
+      <c r="N6" s="85">
+        <v>0</v>
+      </c>
+      <c r="O6" s="85">
+        <v>0</v>
+      </c>
+      <c r="P6" s="85">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="85">
+        <v>0</v>
+      </c>
+      <c r="R6" s="85">
+        <v>0</v>
+      </c>
+      <c r="S6" s="85">
+        <v>0</v>
+      </c>
+      <c r="T6" s="85">
+        <v>0</v>
+      </c>
+      <c r="U6" s="85">
+        <v>0</v>
+      </c>
+      <c r="V6" s="85">
+        <v>0</v>
+      </c>
+      <c r="W6" s="85">
+        <v>0</v>
+      </c>
+      <c r="X6" s="85">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="85">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="185">
         <f>SUM(G6:R6)</f>
         <v>0</v>
       </c>
+      <c r="AF6" s="82"/>
     </row>
     <row r="7" spans="1:33" ht="21" customHeight="1">
-      <c r="A7" s="188"/>
-      <c r="B7" s="65" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="90">
-        <f t="shared" ref="C7:AE7" si="0">SUM(C4:C6)</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="91">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="92">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="91">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Y7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AC7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD7" s="93">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE7" s="189">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AG7" s="82"/>
+      <c r="A7" s="184"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="76">
+        <v>0</v>
+      </c>
+      <c r="D7" s="86">
+        <v>0</v>
+      </c>
+      <c r="E7" s="87">
+        <f>SUM(C7:D7)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="79">
+        <f>SUMIFS($G7:$R7,$G$3:$R$3,"Actuals")</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="88">
+        <v>0</v>
+      </c>
+      <c r="H7" s="89">
+        <v>0</v>
+      </c>
+      <c r="I7" s="89">
+        <v>0</v>
+      </c>
+      <c r="J7" s="89">
+        <v>0</v>
+      </c>
+      <c r="K7" s="89">
+        <v>0</v>
+      </c>
+      <c r="L7" s="89">
+        <v>0</v>
+      </c>
+      <c r="M7" s="89">
+        <v>0</v>
+      </c>
+      <c r="N7" s="89">
+        <v>0</v>
+      </c>
+      <c r="O7" s="89">
+        <v>0</v>
+      </c>
+      <c r="P7" s="89">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="89">
+        <v>0</v>
+      </c>
+      <c r="R7" s="89">
+        <v>0</v>
+      </c>
+      <c r="S7" s="89">
+        <v>0</v>
+      </c>
+      <c r="T7" s="89">
+        <v>0</v>
+      </c>
+      <c r="U7" s="89">
+        <v>0</v>
+      </c>
+      <c r="V7" s="89">
+        <v>0</v>
+      </c>
+      <c r="W7" s="89">
+        <v>0</v>
+      </c>
+      <c r="X7" s="89">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="89">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="89">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="89">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="89">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="89">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="89">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="185">
+        <f>SUM(G7:R7)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:33" ht="21" customHeight="1">
-      <c r="A8" s="190"/>
-      <c r="B8" s="191"/>
-      <c r="C8" s="191"/>
-      <c r="D8" s="191"/>
-      <c r="E8" s="191"/>
-      <c r="F8" s="191"/>
-      <c r="G8" s="192"/>
-      <c r="H8" s="192"/>
-      <c r="I8" s="192"/>
-      <c r="J8" s="192"/>
-      <c r="K8" s="192"/>
-      <c r="L8" s="192"/>
-      <c r="M8" s="192"/>
-      <c r="N8" s="192"/>
-      <c r="O8" s="192"/>
-      <c r="P8" s="192"/>
-      <c r="Q8" s="192"/>
-      <c r="R8" s="192"/>
-      <c r="S8" s="192"/>
-      <c r="T8" s="192"/>
-      <c r="U8" s="192"/>
-      <c r="V8" s="192"/>
-      <c r="W8" s="192"/>
-      <c r="X8" s="192"/>
-      <c r="Y8" s="192"/>
-      <c r="Z8" s="192"/>
-      <c r="AA8" s="192"/>
-      <c r="AB8" s="192"/>
-      <c r="AC8" s="192"/>
-      <c r="AD8" s="192"/>
-      <c r="AE8" s="193"/>
+      <c r="A8" s="186"/>
+      <c r="B8" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="90">
+        <f t="shared" ref="C8:AE8" si="0">SUM(C5:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="91">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="92">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="91">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE8" s="187">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AG8" s="82"/>
     </row>
     <row r="9" spans="1:33" ht="21" customHeight="1">
-      <c r="A9" s="194" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="66" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="94"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="97"/>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="98"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="98"/>
-      <c r="N9" s="98"/>
-      <c r="O9" s="98"/>
-      <c r="P9" s="98"/>
-      <c r="Q9" s="98"/>
-      <c r="R9" s="98"/>
-      <c r="S9" s="98"/>
-      <c r="T9" s="98"/>
-      <c r="U9" s="98"/>
-      <c r="V9" s="98"/>
-      <c r="W9" s="98"/>
-      <c r="X9" s="98"/>
-      <c r="Y9" s="98"/>
-      <c r="Z9" s="98"/>
-      <c r="AA9" s="98"/>
-      <c r="AB9" s="98"/>
-      <c r="AC9" s="98"/>
-      <c r="AD9" s="98"/>
-      <c r="AE9" s="195"/>
+      <c r="A9" s="188"/>
+      <c r="B9" s="189"/>
+      <c r="C9" s="189"/>
+      <c r="D9" s="189"/>
+      <c r="E9" s="189"/>
+      <c r="F9" s="189"/>
+      <c r="G9" s="190"/>
+      <c r="H9" s="190"/>
+      <c r="I9" s="190"/>
+      <c r="J9" s="190"/>
+      <c r="K9" s="190"/>
+      <c r="L9" s="190"/>
+      <c r="M9" s="190"/>
+      <c r="N9" s="190"/>
+      <c r="O9" s="190"/>
+      <c r="P9" s="190"/>
+      <c r="Q9" s="190"/>
+      <c r="R9" s="190"/>
+      <c r="S9" s="190"/>
+      <c r="T9" s="190"/>
+      <c r="U9" s="190"/>
+      <c r="V9" s="190"/>
+      <c r="W9" s="190"/>
+      <c r="X9" s="190"/>
+      <c r="Y9" s="190"/>
+      <c r="Z9" s="190"/>
+      <c r="AA9" s="190"/>
+      <c r="AB9" s="190"/>
+      <c r="AC9" s="190"/>
+      <c r="AD9" s="190"/>
+      <c r="AE9" s="191"/>
     </row>
     <row r="10" spans="1:33" ht="21" customHeight="1">
-      <c r="A10" s="186"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="76">
-        <v>0</v>
-      </c>
-      <c r="D10" s="83">
-        <v>0</v>
-      </c>
-      <c r="E10" s="76">
-        <f>SUM(C10:D10)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="79">
-        <f>SUMIFS($G10:$R10,$G$2:$R$2,"Actuals")</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="80">
-        <v>0</v>
-      </c>
-      <c r="H10" s="81">
-        <v>0</v>
-      </c>
-      <c r="I10" s="81">
-        <v>0</v>
-      </c>
-      <c r="J10" s="81">
-        <v>0</v>
-      </c>
-      <c r="K10" s="81">
-        <v>0</v>
-      </c>
-      <c r="L10" s="81">
-        <v>0</v>
-      </c>
-      <c r="M10" s="81">
-        <v>0</v>
-      </c>
-      <c r="N10" s="81">
-        <v>0</v>
-      </c>
-      <c r="O10" s="81">
-        <v>0</v>
-      </c>
-      <c r="P10" s="81">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="81">
-        <v>0</v>
-      </c>
-      <c r="R10" s="81">
-        <v>0</v>
-      </c>
-      <c r="S10" s="81">
-        <v>0</v>
-      </c>
-      <c r="T10" s="81">
-        <v>0</v>
-      </c>
-      <c r="U10" s="81">
-        <v>0</v>
-      </c>
-      <c r="V10" s="81">
-        <v>0</v>
-      </c>
-      <c r="W10" s="81">
-        <v>0</v>
-      </c>
-      <c r="X10" s="81">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="81">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="81">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="81">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="81">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="81">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="99">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="196">
-        <f>SUM(G10:R10)</f>
-        <v>0</v>
-      </c>
+      <c r="A10" s="192" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="94"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+      <c r="L10" s="98"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="98"/>
+      <c r="O10" s="98"/>
+      <c r="P10" s="98"/>
+      <c r="Q10" s="98"/>
+      <c r="R10" s="98"/>
+      <c r="S10" s="98"/>
+      <c r="T10" s="98"/>
+      <c r="U10" s="98"/>
+      <c r="V10" s="98"/>
+      <c r="W10" s="98"/>
+      <c r="X10" s="98"/>
+      <c r="Y10" s="98"/>
+      <c r="Z10" s="98"/>
+      <c r="AA10" s="98"/>
+      <c r="AB10" s="98"/>
+      <c r="AC10" s="98"/>
+      <c r="AD10" s="98"/>
+      <c r="AE10" s="193"/>
     </row>
     <row r="11" spans="1:33" ht="21" customHeight="1">
-      <c r="A11" s="186"/>
+      <c r="A11" s="184"/>
       <c r="B11" s="67"/>
       <c r="C11" s="76">
         <v>0</v>
@@ -4395,92 +4401,92 @@
         <v>0</v>
       </c>
       <c r="E11" s="76">
-        <f t="shared" ref="E11:E12" si="1">SUM(C11:D11)</f>
+        <f>SUM(C11:D11)</f>
         <v>0</v>
       </c>
       <c r="F11" s="79">
-        <f t="shared" ref="F11:F13" si="2">SUMIFS($G11:$R11,$G$2:$R$2,"Actuals")</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="100">
-        <v>0</v>
-      </c>
-      <c r="H11" s="101">
-        <v>0</v>
-      </c>
-      <c r="I11" s="101">
-        <v>0</v>
-      </c>
-      <c r="J11" s="101">
-        <v>0</v>
-      </c>
-      <c r="K11" s="101">
-        <v>0</v>
-      </c>
-      <c r="L11" s="101">
-        <v>0</v>
-      </c>
-      <c r="M11" s="101">
-        <v>0</v>
-      </c>
-      <c r="N11" s="101">
-        <v>0</v>
-      </c>
-      <c r="O11" s="101">
-        <v>0</v>
-      </c>
-      <c r="P11" s="101">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="101">
-        <v>0</v>
-      </c>
-      <c r="R11" s="101">
-        <v>0</v>
-      </c>
-      <c r="S11" s="101">
-        <v>0</v>
-      </c>
-      <c r="T11" s="101">
-        <v>0</v>
-      </c>
-      <c r="U11" s="101">
-        <v>0</v>
-      </c>
-      <c r="V11" s="101">
-        <v>0</v>
-      </c>
-      <c r="W11" s="101">
-        <v>0</v>
-      </c>
-      <c r="X11" s="101">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="101">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="101">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="101">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="101">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="101">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="102">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="197">
-        <f t="shared" ref="AE11:AE12" si="3">SUM(G11:R11)</f>
+        <f>SUMIFS($G11:$R11,$G$3:$R$3,"Actuals")</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="80">
+        <v>0</v>
+      </c>
+      <c r="H11" s="81">
+        <v>0</v>
+      </c>
+      <c r="I11" s="81">
+        <v>0</v>
+      </c>
+      <c r="J11" s="81">
+        <v>0</v>
+      </c>
+      <c r="K11" s="81">
+        <v>0</v>
+      </c>
+      <c r="L11" s="81">
+        <v>0</v>
+      </c>
+      <c r="M11" s="81">
+        <v>0</v>
+      </c>
+      <c r="N11" s="81">
+        <v>0</v>
+      </c>
+      <c r="O11" s="81">
+        <v>0</v>
+      </c>
+      <c r="P11" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="81">
+        <v>0</v>
+      </c>
+      <c r="R11" s="81">
+        <v>0</v>
+      </c>
+      <c r="S11" s="81">
+        <v>0</v>
+      </c>
+      <c r="T11" s="81">
+        <v>0</v>
+      </c>
+      <c r="U11" s="81">
+        <v>0</v>
+      </c>
+      <c r="V11" s="81">
+        <v>0</v>
+      </c>
+      <c r="W11" s="81">
+        <v>0</v>
+      </c>
+      <c r="X11" s="81">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="81">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="81">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="81">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="81">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="81">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="99">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="194">
+        <f>SUM(G11:R11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:33" ht="21" customHeight="1">
-      <c r="A12" s="186"/>
+      <c r="A12" s="184"/>
       <c r="B12" s="67"/>
       <c r="C12" s="76">
         <v>0</v>
@@ -4489,11 +4495,11 @@
         <v>0</v>
       </c>
       <c r="E12" s="76">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E12:E13" si="1">SUM(C12:D12)</f>
         <v>0</v>
       </c>
       <c r="F12" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F12:F14" si="2">SUMIFS($G12:$R12,$G$3:$R$3,"Actuals")</f>
         <v>0</v>
       </c>
       <c r="G12" s="100">
@@ -4568,13 +4574,13 @@
       <c r="AD12" s="102">
         <v>0</v>
       </c>
-      <c r="AE12" s="197">
-        <f t="shared" si="3"/>
+      <c r="AE12" s="195">
+        <f t="shared" ref="AE12:AE13" si="3">SUM(G12:R12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:33" ht="21" customHeight="1">
-      <c r="A13" s="186"/>
+      <c r="A13" s="184"/>
       <c r="B13" s="67"/>
       <c r="C13" s="76">
         <v>0</v>
@@ -4583,7 +4589,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="76">
-        <f t="shared" ref="E13" si="4">SUM(C13:D13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F13" s="79">
@@ -4662,301 +4668,301 @@
       <c r="AD13" s="102">
         <v>0</v>
       </c>
-      <c r="AE13" s="197">
-        <f t="shared" ref="AE13" si="5">SUM(G13:R13)</f>
+      <c r="AE13" s="195">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="21" customHeight="1">
-      <c r="A14" s="194" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="65" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="90">
-        <f>SUM(C$10:C13)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="91">
-        <f>SUM(D$10:D13)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="92">
-        <f>SUM(E$10:E13)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="91">
-        <f>SUM(F$10:F13)</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="93">
-        <f>SUM(G$10:G13)</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="93">
-        <f>SUM(H$10:H13)</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="93">
-        <f>SUM(I$10:I13)</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="93">
-        <f>SUM(J$10:J13)</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="93">
-        <f>SUM(K$10:K13)</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="93">
-        <f>SUM(L$10:L13)</f>
-        <v>0</v>
-      </c>
-      <c r="M14" s="93">
-        <f>SUM(M$10:M13)</f>
-        <v>0</v>
-      </c>
-      <c r="N14" s="93">
-        <f>SUM(N$10:N13)</f>
-        <v>0</v>
-      </c>
-      <c r="O14" s="93">
-        <f>SUM(O$10:O13)</f>
-        <v>0</v>
-      </c>
-      <c r="P14" s="93">
-        <f>SUM(P$10:P13)</f>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="93">
-        <f>SUM(Q$10:Q13)</f>
-        <v>0</v>
-      </c>
-      <c r="R14" s="93">
-        <f>SUM(R$10:R13)</f>
-        <v>0</v>
-      </c>
-      <c r="S14" s="93">
-        <f>SUM(S$10:S13)</f>
-        <v>0</v>
-      </c>
-      <c r="T14" s="93">
-        <f>SUM(T$10:T13)</f>
-        <v>0</v>
-      </c>
-      <c r="U14" s="93">
-        <f>SUM(U$10:U13)</f>
-        <v>0</v>
-      </c>
-      <c r="V14" s="93">
-        <f>SUM(V$10:V13)</f>
-        <v>0</v>
-      </c>
-      <c r="W14" s="93">
-        <f>SUM(W$10:W13)</f>
-        <v>0</v>
-      </c>
-      <c r="X14" s="93">
-        <f>SUM(X$10:X13)</f>
-        <v>0</v>
-      </c>
-      <c r="Y14" s="93">
-        <f>SUM(Y$10:Y13)</f>
-        <v>0</v>
-      </c>
-      <c r="Z14" s="93">
-        <f>SUM(Z$10:Z13)</f>
-        <v>0</v>
-      </c>
-      <c r="AA14" s="93">
-        <f>SUM(AA$10:AA13)</f>
-        <v>0</v>
-      </c>
-      <c r="AB14" s="93">
-        <f>SUM(AB$10:AB13)</f>
-        <v>0</v>
-      </c>
-      <c r="AC14" s="93">
-        <f>SUM(AC$10:AC13)</f>
-        <v>0</v>
-      </c>
-      <c r="AD14" s="93">
-        <f>SUM(AD$10:AD13)</f>
-        <v>0</v>
-      </c>
-      <c r="AE14" s="189">
-        <f>SUM(AE$10:AE13)</f>
+      <c r="A14" s="184"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="76">
+        <v>0</v>
+      </c>
+      <c r="D14" s="83">
+        <v>0</v>
+      </c>
+      <c r="E14" s="76">
+        <f t="shared" ref="E14" si="4">SUM(C14:D14)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="79">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="100">
+        <v>0</v>
+      </c>
+      <c r="H14" s="101">
+        <v>0</v>
+      </c>
+      <c r="I14" s="101">
+        <v>0</v>
+      </c>
+      <c r="J14" s="101">
+        <v>0</v>
+      </c>
+      <c r="K14" s="101">
+        <v>0</v>
+      </c>
+      <c r="L14" s="101">
+        <v>0</v>
+      </c>
+      <c r="M14" s="101">
+        <v>0</v>
+      </c>
+      <c r="N14" s="101">
+        <v>0</v>
+      </c>
+      <c r="O14" s="101">
+        <v>0</v>
+      </c>
+      <c r="P14" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="101">
+        <v>0</v>
+      </c>
+      <c r="R14" s="101">
+        <v>0</v>
+      </c>
+      <c r="S14" s="101">
+        <v>0</v>
+      </c>
+      <c r="T14" s="101">
+        <v>0</v>
+      </c>
+      <c r="U14" s="101">
+        <v>0</v>
+      </c>
+      <c r="V14" s="101">
+        <v>0</v>
+      </c>
+      <c r="W14" s="101">
+        <v>0</v>
+      </c>
+      <c r="X14" s="101">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="101">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="101">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="101">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="101">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="101">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="102">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="195">
+        <f t="shared" ref="AE14" si="5">SUM(G14:R14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="21" customHeight="1">
-      <c r="A15" s="198"/>
-      <c r="B15" s="191"/>
-      <c r="C15" s="191"/>
-      <c r="D15" s="191"/>
-      <c r="E15" s="191"/>
-      <c r="F15" s="191"/>
-      <c r="G15" s="192"/>
-      <c r="H15" s="192"/>
-      <c r="I15" s="192"/>
-      <c r="J15" s="192"/>
-      <c r="K15" s="192"/>
-      <c r="L15" s="192"/>
-      <c r="M15" s="192"/>
-      <c r="N15" s="192"/>
-      <c r="O15" s="192"/>
-      <c r="P15" s="192"/>
-      <c r="Q15" s="192"/>
-      <c r="R15" s="192"/>
-      <c r="S15" s="192"/>
-      <c r="T15" s="192"/>
-      <c r="U15" s="192"/>
-      <c r="V15" s="192"/>
-      <c r="W15" s="192"/>
-      <c r="X15" s="192"/>
-      <c r="Y15" s="192"/>
-      <c r="Z15" s="192"/>
-      <c r="AA15" s="192"/>
-      <c r="AB15" s="192"/>
-      <c r="AC15" s="192"/>
-      <c r="AD15" s="192"/>
-      <c r="AE15" s="193"/>
+      <c r="A15" s="192" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="90">
+        <f ca="1">SUM(C11:OFFSET(C15, -1, 0))</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="91">
+        <f>SUM(D$11:D14)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="92">
+        <f>SUM(E$11:E14)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="91">
+        <f>SUM(F$11:F14)</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="93">
+        <f>SUM(G$11:G14)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="93">
+        <f>SUM(H$11:H14)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="93">
+        <f>SUM(I$11:I14)</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="93">
+        <f>SUM(J$11:J14)</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="93">
+        <f>SUM(K$11:K14)</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="93">
+        <f>SUM(L$11:L14)</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="93">
+        <f>SUM(M$11:M14)</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="93">
+        <f>SUM(N$11:N14)</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="93">
+        <f>SUM(O$11:O14)</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="93">
+        <f>SUM(P$11:P14)</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="93">
+        <f>SUM(Q$11:Q14)</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="93">
+        <f>SUM(R$11:R14)</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="93">
+        <f>SUM(S$11:S14)</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="93">
+        <f>SUM(T$11:T14)</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="93">
+        <f>SUM(U$11:U14)</f>
+        <v>0</v>
+      </c>
+      <c r="V15" s="93">
+        <f>SUM(V$11:V14)</f>
+        <v>0</v>
+      </c>
+      <c r="W15" s="93">
+        <f>SUM(W$11:W14)</f>
+        <v>0</v>
+      </c>
+      <c r="X15" s="93">
+        <f>SUM(X$11:X14)</f>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="93">
+        <f>SUM(Y$11:Y14)</f>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="93">
+        <f>SUM(Z$11:Z14)</f>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="93">
+        <f>SUM(AA$11:AA14)</f>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="93">
+        <f>SUM(AB$11:AB14)</f>
+        <v>0</v>
+      </c>
+      <c r="AC15" s="93">
+        <f>SUM(AC$11:AC14)</f>
+        <v>0</v>
+      </c>
+      <c r="AD15" s="93">
+        <f>SUM(AD$11:AD14)</f>
+        <v>0</v>
+      </c>
+      <c r="AE15" s="187">
+        <f>SUM(AE$11:AE14)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:33" ht="21" customHeight="1">
-      <c r="A16" s="194" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="66" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="94"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="98"/>
-      <c r="H16" s="98"/>
-      <c r="I16" s="98"/>
-      <c r="J16" s="98"/>
-      <c r="K16" s="98"/>
-      <c r="L16" s="98"/>
-      <c r="M16" s="98"/>
-      <c r="N16" s="98"/>
-      <c r="O16" s="98"/>
-      <c r="P16" s="98"/>
-      <c r="Q16" s="98"/>
-      <c r="R16" s="98"/>
-      <c r="S16" s="98"/>
-      <c r="T16" s="98"/>
-      <c r="U16" s="98"/>
-      <c r="V16" s="98"/>
-      <c r="W16" s="98"/>
-      <c r="X16" s="98"/>
-      <c r="Y16" s="98"/>
-      <c r="Z16" s="98"/>
-      <c r="AA16" s="98"/>
-      <c r="AB16" s="98"/>
-      <c r="AC16" s="98"/>
-      <c r="AD16" s="98"/>
-      <c r="AE16" s="195"/>
+      <c r="A16" s="196"/>
+      <c r="B16" s="189"/>
+      <c r="C16" s="189"/>
+      <c r="D16" s="189"/>
+      <c r="E16" s="189"/>
+      <c r="F16" s="189"/>
+      <c r="G16" s="190"/>
+      <c r="H16" s="190"/>
+      <c r="I16" s="190"/>
+      <c r="J16" s="190"/>
+      <c r="K16" s="190"/>
+      <c r="L16" s="190"/>
+      <c r="M16" s="190"/>
+      <c r="N16" s="190"/>
+      <c r="O16" s="190"/>
+      <c r="P16" s="190"/>
+      <c r="Q16" s="190"/>
+      <c r="R16" s="190"/>
+      <c r="S16" s="190"/>
+      <c r="T16" s="190"/>
+      <c r="U16" s="190"/>
+      <c r="V16" s="190"/>
+      <c r="W16" s="190"/>
+      <c r="X16" s="190"/>
+      <c r="Y16" s="190"/>
+      <c r="Z16" s="190"/>
+      <c r="AA16" s="190"/>
+      <c r="AB16" s="190"/>
+      <c r="AC16" s="190"/>
+      <c r="AD16" s="190"/>
+      <c r="AE16" s="191"/>
     </row>
     <row r="17" spans="1:31" ht="21" customHeight="1">
-      <c r="A17" s="186"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="76">
-        <v>0</v>
-      </c>
-      <c r="D17" s="83">
-        <v>0</v>
-      </c>
-      <c r="E17" s="76">
-        <f t="shared" ref="E17:E20" si="6">SUM(C17:D17)</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="79">
-        <f t="shared" ref="F17:F20" si="7">SUMIFS($G17:$R17,$G$2:$R$2,"Actuals")</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="80">
-        <v>0</v>
-      </c>
-      <c r="H17" s="81">
-        <v>0</v>
-      </c>
-      <c r="I17" s="81">
-        <v>0</v>
-      </c>
-      <c r="J17" s="81">
-        <v>0</v>
-      </c>
-      <c r="K17" s="81">
-        <v>0</v>
-      </c>
-      <c r="L17" s="81">
-        <v>0</v>
-      </c>
-      <c r="M17" s="81">
-        <v>0</v>
-      </c>
-      <c r="N17" s="81">
-        <v>0</v>
-      </c>
-      <c r="O17" s="81">
-        <v>0</v>
-      </c>
-      <c r="P17" s="81">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="81">
-        <v>0</v>
-      </c>
-      <c r="R17" s="81">
-        <v>0</v>
-      </c>
-      <c r="S17" s="81">
-        <v>0</v>
-      </c>
-      <c r="T17" s="81">
-        <v>0</v>
-      </c>
-      <c r="U17" s="81">
-        <v>0</v>
-      </c>
-      <c r="V17" s="81">
-        <v>0</v>
-      </c>
-      <c r="W17" s="81">
-        <v>0</v>
-      </c>
-      <c r="X17" s="81">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="81">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="81">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="81">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="81">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="81">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="99">
-        <v>0</v>
-      </c>
-      <c r="AE17" s="196">
-        <f t="shared" ref="AE17:AE20" si="8">SUM(G17:R17)</f>
-        <v>0</v>
-      </c>
+      <c r="A17" s="192" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="66" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="94"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="97"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="98"/>
+      <c r="I17" s="98"/>
+      <c r="J17" s="98"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="98"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="98"/>
+      <c r="O17" s="98"/>
+      <c r="P17" s="98"/>
+      <c r="Q17" s="98"/>
+      <c r="R17" s="98"/>
+      <c r="S17" s="98"/>
+      <c r="T17" s="98"/>
+      <c r="U17" s="98"/>
+      <c r="V17" s="98"/>
+      <c r="W17" s="98"/>
+      <c r="X17" s="98"/>
+      <c r="Y17" s="98"/>
+      <c r="Z17" s="98"/>
+      <c r="AA17" s="98"/>
+      <c r="AB17" s="98"/>
+      <c r="AC17" s="98"/>
+      <c r="AD17" s="98"/>
+      <c r="AE17" s="193"/>
     </row>
     <row r="18" spans="1:31" ht="21" customHeight="1">
-      <c r="A18" s="186"/>
+      <c r="A18" s="184"/>
       <c r="B18" s="67"/>
       <c r="C18" s="76">
         <v>0</v>
@@ -4965,92 +4971,92 @@
         <v>0</v>
       </c>
       <c r="E18" s="76">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="E18:E21" si="6">SUM(C18:D18)</f>
         <v>0</v>
       </c>
       <c r="F18" s="79">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="100">
-        <v>0</v>
-      </c>
-      <c r="H18" s="101">
-        <v>0</v>
-      </c>
-      <c r="I18" s="101">
-        <v>0</v>
-      </c>
-      <c r="J18" s="101">
-        <v>0</v>
-      </c>
-      <c r="K18" s="101">
-        <v>0</v>
-      </c>
-      <c r="L18" s="101">
-        <v>0</v>
-      </c>
-      <c r="M18" s="101">
-        <v>0</v>
-      </c>
-      <c r="N18" s="101">
-        <v>0</v>
-      </c>
-      <c r="O18" s="101">
-        <v>0</v>
-      </c>
-      <c r="P18" s="101">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="101">
-        <v>0</v>
-      </c>
-      <c r="R18" s="101">
-        <v>0</v>
-      </c>
-      <c r="S18" s="101">
-        <v>0</v>
-      </c>
-      <c r="T18" s="101">
-        <v>0</v>
-      </c>
-      <c r="U18" s="101">
-        <v>0</v>
-      </c>
-      <c r="V18" s="101">
-        <v>0</v>
-      </c>
-      <c r="W18" s="101">
-        <v>0</v>
-      </c>
-      <c r="X18" s="101">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="101">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="101">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="101">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="101">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="101">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="102">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="197">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="F18:F21" si="7">SUMIFS($G18:$R18,$G$3:$R$3,"Actuals")</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="80">
+        <v>0</v>
+      </c>
+      <c r="H18" s="81">
+        <v>0</v>
+      </c>
+      <c r="I18" s="81">
+        <v>0</v>
+      </c>
+      <c r="J18" s="81">
+        <v>0</v>
+      </c>
+      <c r="K18" s="81">
+        <v>0</v>
+      </c>
+      <c r="L18" s="81">
+        <v>0</v>
+      </c>
+      <c r="M18" s="81">
+        <v>0</v>
+      </c>
+      <c r="N18" s="81">
+        <v>0</v>
+      </c>
+      <c r="O18" s="81">
+        <v>0</v>
+      </c>
+      <c r="P18" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="81">
+        <v>0</v>
+      </c>
+      <c r="R18" s="81">
+        <v>0</v>
+      </c>
+      <c r="S18" s="81">
+        <v>0</v>
+      </c>
+      <c r="T18" s="81">
+        <v>0</v>
+      </c>
+      <c r="U18" s="81">
+        <v>0</v>
+      </c>
+      <c r="V18" s="81">
+        <v>0</v>
+      </c>
+      <c r="W18" s="81">
+        <v>0</v>
+      </c>
+      <c r="X18" s="81">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="81">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="81">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="81">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="81">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="81">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="99">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="194">
+        <f t="shared" ref="AE18:AE21" si="8">SUM(G18:R18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="21" customHeight="1">
-      <c r="A19" s="186"/>
+      <c r="A19" s="184"/>
       <c r="B19" s="67"/>
       <c r="C19" s="76">
         <v>0</v>
@@ -5138,13 +5144,13 @@
       <c r="AD19" s="102">
         <v>0</v>
       </c>
-      <c r="AE19" s="197">
+      <c r="AE19" s="195">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="21" customHeight="1">
-      <c r="A20" s="186"/>
+      <c r="A20" s="184"/>
       <c r="B20" s="67"/>
       <c r="C20" s="76">
         <v>0</v>
@@ -5160,871 +5166,990 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G20" s="103">
-        <v>0</v>
-      </c>
-      <c r="H20" s="104">
-        <v>0</v>
-      </c>
-      <c r="I20" s="104">
-        <v>0</v>
-      </c>
-      <c r="J20" s="104">
-        <v>0</v>
-      </c>
-      <c r="K20" s="104">
-        <v>0</v>
-      </c>
-      <c r="L20" s="104">
-        <v>0</v>
-      </c>
-      <c r="M20" s="104">
-        <v>0</v>
-      </c>
-      <c r="N20" s="104">
-        <v>0</v>
-      </c>
-      <c r="O20" s="104">
-        <v>0</v>
-      </c>
-      <c r="P20" s="104">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="104">
-        <v>0</v>
-      </c>
-      <c r="R20" s="104">
-        <v>0</v>
-      </c>
-      <c r="S20" s="104">
-        <v>0</v>
-      </c>
-      <c r="T20" s="104">
-        <v>0</v>
-      </c>
-      <c r="U20" s="104">
-        <v>0</v>
-      </c>
-      <c r="V20" s="104">
-        <v>0</v>
-      </c>
-      <c r="W20" s="104">
-        <v>0</v>
-      </c>
-      <c r="X20" s="104">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="104">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="104">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="104">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="104">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="104">
-        <v>0</v>
-      </c>
-      <c r="AD20" s="105">
-        <v>0</v>
-      </c>
-      <c r="AE20" s="199">
+      <c r="G20" s="100">
+        <v>0</v>
+      </c>
+      <c r="H20" s="101">
+        <v>0</v>
+      </c>
+      <c r="I20" s="101">
+        <v>0</v>
+      </c>
+      <c r="J20" s="101">
+        <v>0</v>
+      </c>
+      <c r="K20" s="101">
+        <v>0</v>
+      </c>
+      <c r="L20" s="101">
+        <v>0</v>
+      </c>
+      <c r="M20" s="101">
+        <v>0</v>
+      </c>
+      <c r="N20" s="101">
+        <v>0</v>
+      </c>
+      <c r="O20" s="101">
+        <v>0</v>
+      </c>
+      <c r="P20" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="101">
+        <v>0</v>
+      </c>
+      <c r="R20" s="101">
+        <v>0</v>
+      </c>
+      <c r="S20" s="101">
+        <v>0</v>
+      </c>
+      <c r="T20" s="101">
+        <v>0</v>
+      </c>
+      <c r="U20" s="101">
+        <v>0</v>
+      </c>
+      <c r="V20" s="101">
+        <v>0</v>
+      </c>
+      <c r="W20" s="101">
+        <v>0</v>
+      </c>
+      <c r="X20" s="101">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="101">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="101">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="101">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="101">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="101">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="102">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="195">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="21" customHeight="1">
-      <c r="A21" s="194" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="90">
-        <f>SUM(C$17:C20)</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="91">
-        <f>SUM(D$17:D20)</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="92">
-        <f>SUM(E$17:E20)</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="91">
-        <f>SUM(F$17:F20)</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="93">
-        <f>SUM(G$17:G20)</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="93">
-        <f>SUM(H$17:H20)</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="93">
-        <f>SUM(I$17:I20)</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="93">
-        <f>SUM(J$17:J20)</f>
-        <v>0</v>
-      </c>
-      <c r="K21" s="93">
-        <f>SUM(K$17:K20)</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="93">
-        <f>SUM(L$17:L20)</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="93">
-        <f>SUM(M$17:M20)</f>
-        <v>0</v>
-      </c>
-      <c r="N21" s="93">
-        <f>SUM(N$17:N20)</f>
-        <v>0</v>
-      </c>
-      <c r="O21" s="93">
-        <f>SUM(O$17:O20)</f>
-        <v>0</v>
-      </c>
-      <c r="P21" s="93">
-        <f>SUM(P$17:P20)</f>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="93">
-        <f>SUM(Q$17:Q20)</f>
-        <v>0</v>
-      </c>
-      <c r="R21" s="93">
-        <f>SUM(R$17:R20)</f>
-        <v>0</v>
-      </c>
-      <c r="S21" s="93">
-        <f>SUM(S$17:S20)</f>
-        <v>0</v>
-      </c>
-      <c r="T21" s="93">
-        <f>SUM(T$17:T20)</f>
-        <v>0</v>
-      </c>
-      <c r="U21" s="93">
-        <f>SUM(U$17:U20)</f>
-        <v>0</v>
-      </c>
-      <c r="V21" s="93">
-        <f>SUM(V$17:V20)</f>
-        <v>0</v>
-      </c>
-      <c r="W21" s="93">
-        <f>SUM(W$17:W20)</f>
-        <v>0</v>
-      </c>
-      <c r="X21" s="93">
-        <f>SUM(X$17:X20)</f>
-        <v>0</v>
-      </c>
-      <c r="Y21" s="93">
-        <f>SUM(Y$17:Y20)</f>
-        <v>0</v>
-      </c>
-      <c r="Z21" s="93">
-        <f>SUM(Z$17:Z20)</f>
-        <v>0</v>
-      </c>
-      <c r="AA21" s="93">
-        <f>SUM(AA$17:AA20)</f>
-        <v>0</v>
-      </c>
-      <c r="AB21" s="93">
-        <f>SUM(AB$17:AB20)</f>
-        <v>0</v>
-      </c>
-      <c r="AC21" s="93">
-        <f>SUM(AC$17:AC20)</f>
-        <v>0</v>
-      </c>
-      <c r="AD21" s="93">
-        <f>SUM(AD$17:AD20)</f>
-        <v>0</v>
-      </c>
-      <c r="AE21" s="189">
-        <f>SUM(AE$17:AE20)</f>
+      <c r="A21" s="184"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="76">
+        <v>0</v>
+      </c>
+      <c r="D21" s="83">
+        <v>0</v>
+      </c>
+      <c r="E21" s="76">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="79">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="103">
+        <v>0</v>
+      </c>
+      <c r="H21" s="104">
+        <v>0</v>
+      </c>
+      <c r="I21" s="104">
+        <v>0</v>
+      </c>
+      <c r="J21" s="104">
+        <v>0</v>
+      </c>
+      <c r="K21" s="104">
+        <v>0</v>
+      </c>
+      <c r="L21" s="104">
+        <v>0</v>
+      </c>
+      <c r="M21" s="104">
+        <v>0</v>
+      </c>
+      <c r="N21" s="104">
+        <v>0</v>
+      </c>
+      <c r="O21" s="104">
+        <v>0</v>
+      </c>
+      <c r="P21" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="104">
+        <v>0</v>
+      </c>
+      <c r="R21" s="104">
+        <v>0</v>
+      </c>
+      <c r="S21" s="104">
+        <v>0</v>
+      </c>
+      <c r="T21" s="104">
+        <v>0</v>
+      </c>
+      <c r="U21" s="104">
+        <v>0</v>
+      </c>
+      <c r="V21" s="104">
+        <v>0</v>
+      </c>
+      <c r="W21" s="104">
+        <v>0</v>
+      </c>
+      <c r="X21" s="104">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="104">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="104">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="104">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="104">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="104">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="105">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="197">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="21" customHeight="1">
-      <c r="A22" s="190"/>
-      <c r="B22" s="191"/>
-      <c r="C22" s="191"/>
-      <c r="D22" s="191"/>
-      <c r="E22" s="191"/>
-      <c r="F22" s="191"/>
-      <c r="G22" s="192"/>
-      <c r="H22" s="192"/>
-      <c r="I22" s="192"/>
-      <c r="J22" s="192"/>
-      <c r="K22" s="192"/>
-      <c r="L22" s="192"/>
-      <c r="M22" s="192"/>
-      <c r="N22" s="192"/>
-      <c r="O22" s="192"/>
-      <c r="P22" s="192"/>
-      <c r="Q22" s="192"/>
-      <c r="R22" s="192"/>
-      <c r="S22" s="192"/>
-      <c r="T22" s="192"/>
-      <c r="U22" s="192"/>
-      <c r="V22" s="192"/>
-      <c r="W22" s="192"/>
-      <c r="X22" s="192"/>
-      <c r="Y22" s="192"/>
-      <c r="Z22" s="192"/>
-      <c r="AA22" s="192"/>
-      <c r="AB22" s="192"/>
-      <c r="AC22" s="192"/>
-      <c r="AD22" s="192"/>
-      <c r="AE22" s="193"/>
+      <c r="A22" s="192" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="90">
+        <f>SUM(C$18:C21)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="91">
+        <f>SUM(D$18:D21)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="92">
+        <f>SUM(E$18:E21)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="91">
+        <f>SUM(F$18:F21)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="93">
+        <f>SUM(G$18:G21)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="93">
+        <f>SUM(H$18:H21)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="93">
+        <f>SUM(I$18:I21)</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="93">
+        <f>SUM(J$18:J21)</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="93">
+        <f>SUM(K$18:K21)</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="93">
+        <f>SUM(L$18:L21)</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="93">
+        <f>SUM(M$18:M21)</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="93">
+        <f>SUM(N$18:N21)</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="93">
+        <f>SUM(O$18:O21)</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="93">
+        <f>SUM(P$18:P21)</f>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="93">
+        <f>SUM(Q$18:Q21)</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="93">
+        <f>SUM(R$18:R21)</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="93">
+        <f>SUM(S$18:S21)</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="93">
+        <f>SUM(T$18:T21)</f>
+        <v>0</v>
+      </c>
+      <c r="U22" s="93">
+        <f>SUM(U$18:U21)</f>
+        <v>0</v>
+      </c>
+      <c r="V22" s="93">
+        <f>SUM(V$18:V21)</f>
+        <v>0</v>
+      </c>
+      <c r="W22" s="93">
+        <f>SUM(W$18:W21)</f>
+        <v>0</v>
+      </c>
+      <c r="X22" s="93">
+        <f>SUM(X$18:X21)</f>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="93">
+        <f>SUM(Y$18:Y21)</f>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="93">
+        <f>SUM(Z$18:Z21)</f>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="93">
+        <f>SUM(AA$18:AA21)</f>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="93">
+        <f>SUM(AB$18:AB21)</f>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="93">
+        <f>SUM(AC$18:AC21)</f>
+        <v>0</v>
+      </c>
+      <c r="AD22" s="93">
+        <f>SUM(AD$18:AD21)</f>
+        <v>0</v>
+      </c>
+      <c r="AE22" s="187">
+        <f>SUM(AE$18:AE21)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:31" ht="21" customHeight="1">
       <c r="A23" s="188"/>
-      <c r="B23" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="90">
-        <f>SUM(C14, C21)</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="91">
-        <f t="shared" ref="D23:AE23" si="9">SUM(D14, D21)</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="92">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="91">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="N23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="S23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="T23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="U23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="V23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="W23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="X23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Y23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Z23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AC23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AD23" s="93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AE23" s="189">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
+      <c r="B23" s="189"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="189"/>
+      <c r="F23" s="189"/>
+      <c r="G23" s="190"/>
+      <c r="H23" s="190"/>
+      <c r="I23" s="190"/>
+      <c r="J23" s="190"/>
+      <c r="K23" s="190"/>
+      <c r="L23" s="190"/>
+      <c r="M23" s="190"/>
+      <c r="N23" s="190"/>
+      <c r="O23" s="190"/>
+      <c r="P23" s="190"/>
+      <c r="Q23" s="190"/>
+      <c r="R23" s="190"/>
+      <c r="S23" s="190"/>
+      <c r="T23" s="190"/>
+      <c r="U23" s="190"/>
+      <c r="V23" s="190"/>
+      <c r="W23" s="190"/>
+      <c r="X23" s="190"/>
+      <c r="Y23" s="190"/>
+      <c r="Z23" s="190"/>
+      <c r="AA23" s="190"/>
+      <c r="AB23" s="190"/>
+      <c r="AC23" s="190"/>
+      <c r="AD23" s="190"/>
+      <c r="AE23" s="191"/>
     </row>
     <row r="24" spans="1:31" ht="21" customHeight="1">
-      <c r="A24" s="190"/>
-      <c r="B24" s="191"/>
-      <c r="C24" s="191"/>
-      <c r="D24" s="191"/>
-      <c r="E24" s="191"/>
-      <c r="F24" s="191"/>
-      <c r="G24" s="192"/>
-      <c r="H24" s="192"/>
-      <c r="I24" s="192"/>
-      <c r="J24" s="192"/>
-      <c r="K24" s="192"/>
-      <c r="L24" s="192"/>
-      <c r="M24" s="192"/>
-      <c r="N24" s="192"/>
-      <c r="O24" s="192"/>
-      <c r="P24" s="192"/>
-      <c r="Q24" s="192"/>
-      <c r="R24" s="192"/>
-      <c r="S24" s="192"/>
-      <c r="T24" s="192"/>
-      <c r="U24" s="192"/>
-      <c r="V24" s="192"/>
-      <c r="W24" s="192"/>
-      <c r="X24" s="192"/>
-      <c r="Y24" s="192"/>
-      <c r="Z24" s="192"/>
-      <c r="AA24" s="192"/>
-      <c r="AB24" s="192"/>
-      <c r="AC24" s="192"/>
-      <c r="AD24" s="192"/>
-      <c r="AE24" s="193"/>
+      <c r="A24" s="186"/>
+      <c r="B24" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="90">
+        <f ca="1">SUM(C15, C22)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="91">
+        <f t="shared" ref="D24:AE24" si="9">SUM(D15, D22)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="92">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="91">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="W24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="X24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AC24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AD24" s="93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE24" s="187">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:31" ht="21" customHeight="1">
       <c r="A25" s="188"/>
-      <c r="B25" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="90">
-        <f>+C7-C23</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="91">
-        <f t="shared" ref="D25:AE25" si="10">+D7-D23</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="92">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="91">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="N25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="O25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="R25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="S25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="T25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="U25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="V25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="W25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Y25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Z25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AA25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AD25" s="93">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AE25" s="189">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="B25" s="189"/>
+      <c r="C25" s="189"/>
+      <c r="D25" s="189"/>
+      <c r="E25" s="189"/>
+      <c r="F25" s="189"/>
+      <c r="G25" s="190"/>
+      <c r="H25" s="190"/>
+      <c r="I25" s="190"/>
+      <c r="J25" s="190"/>
+      <c r="K25" s="190"/>
+      <c r="L25" s="190"/>
+      <c r="M25" s="190"/>
+      <c r="N25" s="190"/>
+      <c r="O25" s="190"/>
+      <c r="P25" s="190"/>
+      <c r="Q25" s="190"/>
+      <c r="R25" s="190"/>
+      <c r="S25" s="190"/>
+      <c r="T25" s="190"/>
+      <c r="U25" s="190"/>
+      <c r="V25" s="190"/>
+      <c r="W25" s="190"/>
+      <c r="X25" s="190"/>
+      <c r="Y25" s="190"/>
+      <c r="Z25" s="190"/>
+      <c r="AA25" s="190"/>
+      <c r="AB25" s="190"/>
+      <c r="AC25" s="190"/>
+      <c r="AD25" s="190"/>
+      <c r="AE25" s="191"/>
     </row>
     <row r="26" spans="1:31" ht="21" customHeight="1">
-      <c r="A26" s="190"/>
-      <c r="B26" s="191"/>
-      <c r="C26" s="191"/>
-      <c r="D26" s="191"/>
-      <c r="E26" s="191"/>
-      <c r="F26" s="191"/>
-      <c r="G26" s="192"/>
-      <c r="H26" s="192"/>
-      <c r="I26" s="192"/>
-      <c r="J26" s="192"/>
-      <c r="K26" s="192"/>
-      <c r="L26" s="192"/>
-      <c r="M26" s="192"/>
-      <c r="N26" s="192"/>
-      <c r="O26" s="192"/>
-      <c r="P26" s="192"/>
-      <c r="Q26" s="192"/>
-      <c r="R26" s="192"/>
-      <c r="S26" s="192"/>
-      <c r="T26" s="192"/>
-      <c r="U26" s="192"/>
-      <c r="V26" s="192"/>
-      <c r="W26" s="192"/>
-      <c r="X26" s="192"/>
-      <c r="Y26" s="192"/>
-      <c r="Z26" s="192"/>
-      <c r="AA26" s="192"/>
-      <c r="AB26" s="192"/>
-      <c r="AC26" s="192"/>
-      <c r="AD26" s="192"/>
-      <c r="AE26" s="193"/>
+      <c r="A26" s="186"/>
+      <c r="B26" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="90">
+        <f ca="1">+C8-C24</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="91">
+        <f t="shared" ref="D26:AE26" si="10">+D8-D24</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="92">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="91">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="S26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="T26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="U26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Z26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AB26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AC26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AD26" s="93">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AE26" s="187">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:31" ht="21" customHeight="1">
       <c r="A27" s="188"/>
-      <c r="B27" s="70" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="94"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="96"/>
-      <c r="F27" s="97"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="98"/>
-      <c r="I27" s="98"/>
-      <c r="J27" s="98"/>
-      <c r="K27" s="98"/>
-      <c r="L27" s="98"/>
-      <c r="M27" s="98"/>
-      <c r="N27" s="98"/>
-      <c r="O27" s="98"/>
-      <c r="P27" s="98"/>
-      <c r="Q27" s="98"/>
-      <c r="R27" s="98"/>
-      <c r="S27" s="98"/>
-      <c r="T27" s="98"/>
-      <c r="U27" s="98"/>
-      <c r="V27" s="98"/>
-      <c r="W27" s="98"/>
-      <c r="X27" s="98"/>
-      <c r="Y27" s="98"/>
-      <c r="Z27" s="98"/>
-      <c r="AA27" s="98"/>
-      <c r="AB27" s="98"/>
-      <c r="AC27" s="98"/>
-      <c r="AD27" s="98"/>
-      <c r="AE27" s="195"/>
+      <c r="B27" s="189"/>
+      <c r="C27" s="189"/>
+      <c r="D27" s="189"/>
+      <c r="E27" s="189"/>
+      <c r="F27" s="189"/>
+      <c r="G27" s="190"/>
+      <c r="H27" s="190"/>
+      <c r="I27" s="190"/>
+      <c r="J27" s="190"/>
+      <c r="K27" s="190"/>
+      <c r="L27" s="190"/>
+      <c r="M27" s="190"/>
+      <c r="N27" s="190"/>
+      <c r="O27" s="190"/>
+      <c r="P27" s="190"/>
+      <c r="Q27" s="190"/>
+      <c r="R27" s="190"/>
+      <c r="S27" s="190"/>
+      <c r="T27" s="190"/>
+      <c r="U27" s="190"/>
+      <c r="V27" s="190"/>
+      <c r="W27" s="190"/>
+      <c r="X27" s="190"/>
+      <c r="Y27" s="190"/>
+      <c r="Z27" s="190"/>
+      <c r="AA27" s="190"/>
+      <c r="AB27" s="190"/>
+      <c r="AC27" s="190"/>
+      <c r="AD27" s="190"/>
+      <c r="AE27" s="191"/>
     </row>
     <row r="28" spans="1:31" ht="21" customHeight="1">
-      <c r="A28" s="200"/>
-      <c r="B28" s="69" t="s">
+      <c r="A28" s="186"/>
+      <c r="B28" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="94"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="97"/>
+      <c r="G28" s="98"/>
+      <c r="H28" s="98"/>
+      <c r="I28" s="98"/>
+      <c r="J28" s="98"/>
+      <c r="K28" s="98"/>
+      <c r="L28" s="98"/>
+      <c r="M28" s="98"/>
+      <c r="N28" s="98"/>
+      <c r="O28" s="98"/>
+      <c r="P28" s="98"/>
+      <c r="Q28" s="98"/>
+      <c r="R28" s="98"/>
+      <c r="S28" s="98"/>
+      <c r="T28" s="98"/>
+      <c r="U28" s="98"/>
+      <c r="V28" s="98"/>
+      <c r="W28" s="98"/>
+      <c r="X28" s="98"/>
+      <c r="Y28" s="98"/>
+      <c r="Z28" s="98"/>
+      <c r="AA28" s="98"/>
+      <c r="AB28" s="98"/>
+      <c r="AC28" s="98"/>
+      <c r="AD28" s="98"/>
+      <c r="AE28" s="193"/>
+    </row>
+    <row r="29" spans="1:31" ht="21" customHeight="1">
+      <c r="A29" s="198"/>
+      <c r="B29" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="180" t="e">
-        <f>+C14/C7</f>
+      <c r="C29" s="180" t="e">
+        <f ca="1">+C15/C8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D28" s="180" t="e">
-        <f t="shared" ref="D28:AD28" si="11">+D14/D7</f>
+      <c r="D29" s="180" t="e">
+        <f t="shared" ref="D29:AD29" si="11">+D15/D8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E28" s="180" t="e">
+      <c r="E29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F28" s="180" t="e">
+      <c r="F29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G28" s="180" t="e">
+      <c r="G29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H28" s="180" t="e">
+      <c r="H29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I28" s="180" t="e">
+      <c r="I29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J28" s="180" t="e">
+      <c r="J29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K28" s="180" t="e">
+      <c r="K29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L28" s="180" t="e">
+      <c r="L29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M28" s="180" t="e">
+      <c r="M29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N28" s="180" t="e">
+      <c r="N29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O28" s="180" t="e">
+      <c r="O29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P28" s="180" t="e">
+      <c r="P29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q28" s="180" t="e">
+      <c r="Q29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R28" s="180" t="e">
+      <c r="R29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S28" s="180" t="e">
+      <c r="S29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T28" s="180" t="e">
+      <c r="T29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U28" s="180" t="e">
+      <c r="U29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="V28" s="180" t="e">
+      <c r="V29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="W28" s="180" t="e">
+      <c r="W29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X28" s="180" t="e">
+      <c r="X29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y28" s="180" t="e">
+      <c r="Y29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z28" s="180" t="e">
+      <c r="Z29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA28" s="180" t="e">
+      <c r="AA29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AB28" s="180" t="e">
+      <c r="AB29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC28" s="180" t="e">
+      <c r="AC29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD28" s="180" t="e">
+      <c r="AD29" s="180" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE28" s="201" t="e">
-        <f t="shared" ref="AE28" si="12">+AE14/AE7</f>
+      <c r="AE29" s="199" t="e">
+        <f t="shared" ref="AE29" si="12">+AE15/AE8</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="21" customHeight="1">
-      <c r="A29" s="200"/>
-      <c r="B29" s="69" t="s">
+    <row r="30" spans="1:31" ht="21" customHeight="1">
+      <c r="A30" s="198"/>
+      <c r="B30" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="180" t="e">
-        <f>+C21/C7</f>
+      <c r="C30" s="180" t="e">
+        <f>+C22/C8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D29" s="180" t="e">
-        <f t="shared" ref="D29:AD29" si="13">+D21/D7</f>
+      <c r="D30" s="180" t="e">
+        <f t="shared" ref="D30:AD30" si="13">+D22/D8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E29" s="180" t="e">
+      <c r="E30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F29" s="180" t="e">
+      <c r="F30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G29" s="180" t="e">
+      <c r="G30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H29" s="180" t="e">
+      <c r="H30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I29" s="180" t="e">
+      <c r="I30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J29" s="180" t="e">
+      <c r="J30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K29" s="180" t="e">
+      <c r="K30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L29" s="180" t="e">
+      <c r="L30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M29" s="180" t="e">
+      <c r="M30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N29" s="180" t="e">
+      <c r="N30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O29" s="180" t="e">
+      <c r="O30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P29" s="180" t="e">
+      <c r="P30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q29" s="180" t="e">
+      <c r="Q30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R29" s="180" t="e">
+      <c r="R30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S29" s="180" t="e">
+      <c r="S30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T29" s="180" t="e">
+      <c r="T30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U29" s="180" t="e">
+      <c r="U30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="V29" s="180" t="e">
+      <c r="V30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="W29" s="180" t="e">
+      <c r="W30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X29" s="180" t="e">
+      <c r="X30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y29" s="180" t="e">
+      <c r="Y30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z29" s="180" t="e">
+      <c r="Z30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA29" s="180" t="e">
+      <c r="AA30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AB29" s="180" t="e">
+      <c r="AB30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC29" s="180" t="e">
+      <c r="AC30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD29" s="180" t="e">
+      <c r="AD30" s="180" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE29" s="201" t="e">
-        <f t="shared" ref="AE29" si="14">+AE21/AE7</f>
+      <c r="AE30" s="199" t="e">
+        <f t="shared" ref="AE30" si="14">+AE22/AE8</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="21" customHeight="1" thickBot="1">
-      <c r="A30" s="202"/>
-      <c r="B30" s="203" t="s">
+    <row r="31" spans="1:31" ht="21" customHeight="1" thickBot="1">
+      <c r="A31" s="200"/>
+      <c r="B31" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="204"/>
-      <c r="D30" s="205"/>
-      <c r="E30" s="206"/>
-      <c r="F30" s="207"/>
-      <c r="G30" s="208"/>
-      <c r="H30" s="208"/>
-      <c r="I30" s="208"/>
-      <c r="J30" s="208"/>
-      <c r="K30" s="208"/>
-      <c r="L30" s="208"/>
-      <c r="M30" s="208"/>
-      <c r="N30" s="208"/>
-      <c r="O30" s="208"/>
-      <c r="P30" s="208"/>
-      <c r="Q30" s="208"/>
-      <c r="R30" s="208"/>
-      <c r="S30" s="208"/>
-      <c r="T30" s="208"/>
-      <c r="U30" s="208"/>
-      <c r="V30" s="208"/>
-      <c r="W30" s="208"/>
-      <c r="X30" s="208"/>
-      <c r="Y30" s="208"/>
-      <c r="Z30" s="208"/>
-      <c r="AA30" s="208"/>
-      <c r="AB30" s="208"/>
-      <c r="AC30" s="208"/>
-      <c r="AD30" s="208"/>
-      <c r="AE30" s="209"/>
+      <c r="C31" s="202"/>
+      <c r="D31" s="203"/>
+      <c r="E31" s="204"/>
+      <c r="F31" s="205"/>
+      <c r="G31" s="206"/>
+      <c r="H31" s="206"/>
+      <c r="I31" s="206"/>
+      <c r="J31" s="206"/>
+      <c r="K31" s="206"/>
+      <c r="L31" s="206"/>
+      <c r="M31" s="206"/>
+      <c r="N31" s="206"/>
+      <c r="O31" s="206"/>
+      <c r="P31" s="206"/>
+      <c r="Q31" s="206"/>
+      <c r="R31" s="206"/>
+      <c r="S31" s="206"/>
+      <c r="T31" s="206"/>
+      <c r="U31" s="206"/>
+      <c r="V31" s="206"/>
+      <c r="W31" s="206"/>
+      <c r="X31" s="206"/>
+      <c r="Y31" s="206"/>
+      <c r="Z31" s="206"/>
+      <c r="AA31" s="206"/>
+      <c r="AB31" s="206"/>
+      <c r="AC31" s="206"/>
+      <c r="AD31" s="206"/>
+      <c r="AE31" s="207"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A2:B2"/>
+  <mergeCells count="28">
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:E3">
+  <conditionalFormatting sqref="C4:E4">
     <cfRule type="cellIs" dxfId="3" priority="39" operator="equal">
       <formula>"ERROR"</formula>
     </cfRule>
@@ -6063,16 +6188,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="21" customHeight="1">
-      <c r="A1" s="218" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="219"/>
-      <c r="C1" s="222" t="s">
+      <c r="A1" s="224" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="225"/>
+      <c r="C1" s="228" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="215"/>
-      <c r="E1" s="215"/>
-      <c r="F1" s="223"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="229"/>
       <c r="G1" s="58">
         <v>43556</v>
       </c>
@@ -6114,8 +6239,8 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="A2" s="220"/>
-      <c r="B2" s="221"/>
+      <c r="A2" s="226"/>
+      <c r="B2" s="227"/>
       <c r="C2" s="106" t="s">
         <v>3</v>
       </c>
@@ -6173,9 +6298,9 @@
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
+      <c r="C3" s="230"/>
+      <c r="D3" s="211"/>
+      <c r="E3" s="211"/>
       <c r="F3" s="5"/>
       <c r="G3" s="109"/>
       <c r="H3" s="109"/>

</xml_diff>